<commit_message>
Pflichtenheft zusammengefasst und Gantt erweitert
</commit_message>
<xml_diff>
--- a/Projektplanung/Gantt-Diagramm.xlsx
+++ b/Projektplanung/Gantt-Diagramm.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4040E4B-6CB7-431C-9066-838F9711C52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B4E1A-6002-4B49-8FFB-5AE2AE3D8008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1239,12 +1239,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1256,6 +1250,12 @@
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1649,7 +1649,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$E$4" horiz="1" max="100" page="0" val="8"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$E$4" horiz="1" max="100" page="0" val="12"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2049,8 +2049,8 @@
   <dimension ref="A1:CP48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2097,14 +2097,14 @@
       <c r="B3" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="60">
+      <c r="D3" s="60"/>
+      <c r="E3" s="58">
         <v>45819</v>
       </c>
-      <c r="F3" s="60"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2113,93 +2113,93 @@
       <c r="B4" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="7">
-        <v>8</v>
-      </c>
-      <c r="I4" s="57">
+        <v>12</v>
+      </c>
+      <c r="I4" s="55">
         <f>I5</f>
-        <v>45866</v>
-      </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="57">
+        <v>45894</v>
+      </c>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="55">
         <f>P5</f>
-        <v>45873</v>
-      </c>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="57">
+        <v>45901</v>
+      </c>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="55">
         <f>W5</f>
-        <v>45880</v>
-      </c>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="57">
+        <v>45908</v>
+      </c>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="56"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="55">
         <f>AD5</f>
-        <v>45887</v>
-      </c>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="57">
+        <v>45915</v>
+      </c>
+      <c r="AE4" s="56"/>
+      <c r="AF4" s="56"/>
+      <c r="AG4" s="56"/>
+      <c r="AH4" s="56"/>
+      <c r="AI4" s="56"/>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="55">
         <f>AK5</f>
-        <v>45894</v>
-      </c>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="58"/>
-      <c r="AN4" s="58"/>
-      <c r="AO4" s="58"/>
-      <c r="AP4" s="58"/>
-      <c r="AQ4" s="59"/>
-      <c r="AR4" s="57">
+        <v>45922</v>
+      </c>
+      <c r="AL4" s="56"/>
+      <c r="AM4" s="56"/>
+      <c r="AN4" s="56"/>
+      <c r="AO4" s="56"/>
+      <c r="AP4" s="56"/>
+      <c r="AQ4" s="57"/>
+      <c r="AR4" s="55">
         <f>AR5</f>
-        <v>45901</v>
-      </c>
-      <c r="AS4" s="58"/>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="58"/>
-      <c r="AV4" s="58"/>
-      <c r="AW4" s="58"/>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="57">
+        <v>45929</v>
+      </c>
+      <c r="AS4" s="56"/>
+      <c r="AT4" s="56"/>
+      <c r="AU4" s="56"/>
+      <c r="AV4" s="56"/>
+      <c r="AW4" s="56"/>
+      <c r="AX4" s="57"/>
+      <c r="AY4" s="55">
         <f>AY5</f>
-        <v>45908</v>
-      </c>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="58"/>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="58"/>
-      <c r="BD4" s="58"/>
-      <c r="BE4" s="59"/>
-      <c r="BF4" s="57">
+        <v>45936</v>
+      </c>
+      <c r="AZ4" s="56"/>
+      <c r="BA4" s="56"/>
+      <c r="BB4" s="56"/>
+      <c r="BC4" s="56"/>
+      <c r="BD4" s="56"/>
+      <c r="BE4" s="57"/>
+      <c r="BF4" s="55">
         <f>BF5</f>
-        <v>45915</v>
-      </c>
-      <c r="BG4" s="58"/>
-      <c r="BH4" s="58"/>
-      <c r="BI4" s="58"/>
-      <c r="BJ4" s="58"/>
-      <c r="BK4" s="58"/>
-      <c r="BL4" s="59"/>
+        <v>45943</v>
+      </c>
+      <c r="BG4" s="56"/>
+      <c r="BH4" s="56"/>
+      <c r="BI4" s="56"/>
+      <c r="BJ4" s="56"/>
+      <c r="BK4" s="56"/>
+      <c r="BL4" s="57"/>
     </row>
     <row r="5" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -2213,227 +2213,227 @@
       <c r="G5" s="40"/>
       <c r="I5" s="47">
         <f>Projektanfang-WEEKDAY(Projektanfang,1)+2+7*(Anzeigewoche-1)</f>
-        <v>45866</v>
+        <v>45894</v>
       </c>
       <c r="J5" s="48">
         <f>I5+1</f>
-        <v>45867</v>
+        <v>45895</v>
       </c>
       <c r="K5" s="48">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>45868</v>
+        <v>45896</v>
       </c>
       <c r="L5" s="48">
         <f t="shared" si="0"/>
-        <v>45869</v>
+        <v>45897</v>
       </c>
       <c r="M5" s="48">
         <f t="shared" si="0"/>
-        <v>45870</v>
+        <v>45898</v>
       </c>
       <c r="N5" s="48">
         <f t="shared" si="0"/>
-        <v>45871</v>
+        <v>45899</v>
       </c>
       <c r="O5" s="49">
         <f t="shared" si="0"/>
-        <v>45872</v>
+        <v>45900</v>
       </c>
       <c r="P5" s="47">
         <f>O5+1</f>
-        <v>45873</v>
+        <v>45901</v>
       </c>
       <c r="Q5" s="48">
         <f>P5+1</f>
-        <v>45874</v>
+        <v>45902</v>
       </c>
       <c r="R5" s="48">
         <f t="shared" si="0"/>
-        <v>45875</v>
+        <v>45903</v>
       </c>
       <c r="S5" s="48">
         <f t="shared" si="0"/>
-        <v>45876</v>
+        <v>45904</v>
       </c>
       <c r="T5" s="48">
         <f t="shared" si="0"/>
-        <v>45877</v>
+        <v>45905</v>
       </c>
       <c r="U5" s="48">
         <f t="shared" si="0"/>
-        <v>45878</v>
+        <v>45906</v>
       </c>
       <c r="V5" s="49">
         <f t="shared" si="0"/>
-        <v>45879</v>
+        <v>45907</v>
       </c>
       <c r="W5" s="47">
         <f>V5+1</f>
-        <v>45880</v>
+        <v>45908</v>
       </c>
       <c r="X5" s="48">
         <f>W5+1</f>
-        <v>45881</v>
+        <v>45909</v>
       </c>
       <c r="Y5" s="48">
         <f t="shared" si="0"/>
-        <v>45882</v>
+        <v>45910</v>
       </c>
       <c r="Z5" s="48">
         <f t="shared" si="0"/>
-        <v>45883</v>
+        <v>45911</v>
       </c>
       <c r="AA5" s="48">
         <f t="shared" si="0"/>
-        <v>45884</v>
+        <v>45912</v>
       </c>
       <c r="AB5" s="48">
         <f t="shared" si="0"/>
-        <v>45885</v>
+        <v>45913</v>
       </c>
       <c r="AC5" s="49">
         <f t="shared" si="0"/>
-        <v>45886</v>
+        <v>45914</v>
       </c>
       <c r="AD5" s="47">
         <f>AC5+1</f>
-        <v>45887</v>
+        <v>45915</v>
       </c>
       <c r="AE5" s="48">
         <f>AD5+1</f>
-        <v>45888</v>
+        <v>45916</v>
       </c>
       <c r="AF5" s="48">
         <f t="shared" si="0"/>
-        <v>45889</v>
+        <v>45917</v>
       </c>
       <c r="AG5" s="48">
         <f t="shared" si="0"/>
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="AH5" s="48">
         <f t="shared" si="0"/>
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="AI5" s="48">
         <f t="shared" si="0"/>
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="AJ5" s="49">
         <f t="shared" si="0"/>
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="AK5" s="47">
         <f>AJ5+1</f>
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="AL5" s="48">
         <f>AK5+1</f>
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="AM5" s="48">
         <f t="shared" si="0"/>
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="AN5" s="48">
         <f t="shared" si="0"/>
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="AO5" s="48">
         <f t="shared" si="0"/>
-        <v>45898</v>
+        <v>45926</v>
       </c>
       <c r="AP5" s="48">
         <f t="shared" si="0"/>
-        <v>45899</v>
+        <v>45927</v>
       </c>
       <c r="AQ5" s="49">
         <f t="shared" si="0"/>
-        <v>45900</v>
+        <v>45928</v>
       </c>
       <c r="AR5" s="47">
         <f>AQ5+1</f>
-        <v>45901</v>
+        <v>45929</v>
       </c>
       <c r="AS5" s="48">
         <f>AR5+1</f>
-        <v>45902</v>
+        <v>45930</v>
       </c>
       <c r="AT5" s="48">
         <f t="shared" si="0"/>
-        <v>45903</v>
+        <v>45931</v>
       </c>
       <c r="AU5" s="48">
         <f t="shared" si="0"/>
-        <v>45904</v>
+        <v>45932</v>
       </c>
       <c r="AV5" s="48">
         <f t="shared" si="0"/>
-        <v>45905</v>
+        <v>45933</v>
       </c>
       <c r="AW5" s="48">
         <f t="shared" si="0"/>
-        <v>45906</v>
+        <v>45934</v>
       </c>
       <c r="AX5" s="49">
         <f t="shared" si="0"/>
-        <v>45907</v>
+        <v>45935</v>
       </c>
       <c r="AY5" s="47">
         <f>AX5+1</f>
-        <v>45908</v>
+        <v>45936</v>
       </c>
       <c r="AZ5" s="48">
         <f>AY5+1</f>
-        <v>45909</v>
+        <v>45937</v>
       </c>
       <c r="BA5" s="48">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45910</v>
+        <v>45938</v>
       </c>
       <c r="BB5" s="48">
         <f t="shared" si="1"/>
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="BC5" s="48">
         <f t="shared" si="1"/>
-        <v>45912</v>
+        <v>45940</v>
       </c>
       <c r="BD5" s="48">
         <f t="shared" si="1"/>
-        <v>45913</v>
+        <v>45941</v>
       </c>
       <c r="BE5" s="49">
         <f t="shared" si="1"/>
-        <v>45914</v>
+        <v>45942</v>
       </c>
       <c r="BF5" s="47">
         <f>BE5+1</f>
-        <v>45915</v>
+        <v>45943</v>
       </c>
       <c r="BG5" s="48">
         <f>BF5+1</f>
-        <v>45916</v>
+        <v>45944</v>
       </c>
       <c r="BH5" s="48">
         <f t="shared" ref="BH5:BK5" si="2">BG5+1</f>
-        <v>45917</v>
+        <v>45945</v>
       </c>
       <c r="BI5" s="48">
         <f t="shared" si="2"/>
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="BJ5" s="48">
         <f t="shared" si="2"/>
-        <v>45919</v>
+        <v>45947</v>
       </c>
       <c r="BK5" s="48">
         <f t="shared" si="2"/>
-        <v>45920</v>
+        <v>45948</v>
       </c>
       <c r="BL5" s="49">
         <f>BK5+1</f>
-        <v>45921</v>
+        <v>45949</v>
       </c>
     </row>
     <row r="6" spans="1:94" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3205,7 +3205,7 @@
         <v>41</v>
       </c>
       <c r="D12" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E12" s="44">
         <f>F11</f>
@@ -4722,7 +4722,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E26" s="44">
         <v>45892</v>
@@ -6853,17 +6853,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D45">
     <cfRule type="dataBar" priority="26">
@@ -6899,7 +6899,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -7066,6 +7066,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
+    <_activity xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EDB812BAF41ADA4394A8076EA0B61C5B" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2edf200c4005839e532231d45070b11f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1386928-745a-4956-98a1-a16a4dd5b026" xmlns:ns4="135f4629-4c69-42bd-b907-0ef6c8daac89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbaa874e3aed9a9139054fcecbe44b3c" ns3:_="" ns4:_="">
     <xsd:import namespace="a1386928-745a-4956-98a1-a16a4dd5b026"/>
@@ -7312,39 +7330,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
-    <_activity xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7D7F31-B484-4E45-8243-CE827741D3B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1386928-745a-4956-98a1-a16a4dd5b026"/>
-    <ds:schemaRef ds:uri="135f4629-4c69-42bd-b907-0ef6c8daac89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7367,9 +7356,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7D7F31-B484-4E45-8243-CE827741D3B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1386928-745a-4956-98a1-a16a4dd5b026"/>
+    <ds:schemaRef ds:uri="135f4629-4c69-42bd-b907-0ef6c8daac89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Recherche Upload und Gantt
</commit_message>
<xml_diff>
--- a/Projektplanung/Gantt-Diagramm.xlsx
+++ b/Projektplanung/Gantt-Diagramm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B4E1A-6002-4B49-8FFB-5AE2AE3D8008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485C174-EE1F-4D01-9755-40B17738470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>6, Wissenschaftliche Arbeit schreiben</t>
-  </si>
-  <si>
-    <t>7, Organigramm erstellen</t>
   </si>
   <si>
     <t>8, Recherche der C# Frameworks</t>
@@ -1239,6 +1236,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1250,12 +1253,6 @@
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1764,10 +1761,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB052DBC-397C-4448-B920-A158FFCAC0DC}" name="Tabelle1" displayName="Tabelle1" ref="B6:F44" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="B6:F44" xr:uid="{DB052DBC-397C-4448-B920-A158FFCAC0DC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:F44">
-    <sortCondition ref="E6:E44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB052DBC-397C-4448-B920-A158FFCAC0DC}" name="Tabelle1" displayName="Tabelle1" ref="B6:F43" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B6:F43" xr:uid="{DB052DBC-397C-4448-B920-A158FFCAC0DC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:F43">
+    <sortCondition ref="E6:E43"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{26835AC6-C1A0-4B24-87CB-3F5A7E96CA81}" name="AUFGABE" dataDxfId="7" dataCellStyle="Aufgabe"/>
@@ -2046,11 +2043,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CP48"/>
+  <dimension ref="A1:CP47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2097,14 +2094,14 @@
       <c r="B3" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="58">
+      <c r="D3" s="56"/>
+      <c r="E3" s="60">
         <v>45819</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2113,93 +2110,93 @@
       <c r="B4" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="7">
         <v>12</v>
       </c>
-      <c r="I4" s="55">
+      <c r="I4" s="57">
         <f>I5</f>
         <v>45894</v>
       </c>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="55">
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="57">
         <f>P5</f>
         <v>45901</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="55">
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="57">
         <f>W5</f>
         <v>45908</v>
       </c>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="56"/>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="55">
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="57">
         <f>AD5</f>
         <v>45915</v>
       </c>
-      <c r="AE4" s="56"/>
-      <c r="AF4" s="56"/>
-      <c r="AG4" s="56"/>
-      <c r="AH4" s="56"/>
-      <c r="AI4" s="56"/>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="55">
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="57">
         <f>AK5</f>
         <v>45922</v>
       </c>
-      <c r="AL4" s="56"/>
-      <c r="AM4" s="56"/>
-      <c r="AN4" s="56"/>
-      <c r="AO4" s="56"/>
-      <c r="AP4" s="56"/>
-      <c r="AQ4" s="57"/>
-      <c r="AR4" s="55">
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="58"/>
+      <c r="AP4" s="58"/>
+      <c r="AQ4" s="59"/>
+      <c r="AR4" s="57">
         <f>AR5</f>
         <v>45929</v>
       </c>
-      <c r="AS4" s="56"/>
-      <c r="AT4" s="56"/>
-      <c r="AU4" s="56"/>
-      <c r="AV4" s="56"/>
-      <c r="AW4" s="56"/>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="55">
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="58"/>
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="57">
         <f>AY5</f>
         <v>45936</v>
       </c>
-      <c r="AZ4" s="56"/>
-      <c r="BA4" s="56"/>
-      <c r="BB4" s="56"/>
-      <c r="BC4" s="56"/>
-      <c r="BD4" s="56"/>
-      <c r="BE4" s="57"/>
-      <c r="BF4" s="55">
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="58"/>
+      <c r="BE4" s="59"/>
+      <c r="BF4" s="57">
         <f>BF5</f>
         <v>45943</v>
       </c>
-      <c r="BG4" s="56"/>
-      <c r="BH4" s="56"/>
-      <c r="BI4" s="56"/>
-      <c r="BJ4" s="56"/>
-      <c r="BK4" s="56"/>
-      <c r="BL4" s="57"/>
+      <c r="BG4" s="58"/>
+      <c r="BH4" s="58"/>
+      <c r="BI4" s="58"/>
+      <c r="BJ4" s="58"/>
+      <c r="BK4" s="58"/>
+      <c r="BL4" s="59"/>
     </row>
     <row r="5" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -2773,7 +2770,7 @@
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12">
-        <f t="shared" ref="H8:H45" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H44" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>3</v>
       </c>
       <c r="I8" s="18"/>
@@ -3310,7 +3307,7 @@
     <row r="13" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32"/>
       <c r="B13" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>48</v>
@@ -3421,7 +3418,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>48</v>
@@ -3530,7 +3527,7 @@
     <row r="15" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
       <c r="B15" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="39" t="s">
         <v>48</v>
@@ -3639,7 +3636,7 @@
     <row r="16" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32"/>
       <c r="B16" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="39" t="s">
         <v>48</v>
@@ -3748,7 +3745,7 @@
     <row r="17" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32"/>
       <c r="B17" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="39" t="s">
         <v>48</v>
@@ -3857,7 +3854,7 @@
     <row r="18" spans="1:94" s="3" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32"/>
       <c r="B18" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="39" t="s">
         <v>47</v>
@@ -3966,7 +3963,7 @@
     <row r="19" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32"/>
       <c r="B19" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>47</v>
@@ -4075,7 +4072,7 @@
     <row r="20" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
       <c r="B20" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="39" t="s">
         <v>47</v>
@@ -4181,7 +4178,7 @@
     <row r="21" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32"/>
       <c r="B21" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>47</v>
@@ -4719,21 +4716,21 @@
         <v>56</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D26" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="44">
-        <v>45892</v>
+        <v>45895</v>
       </c>
       <c r="F26" s="44">
-        <v>45895</v>
+        <v>45899</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
@@ -4825,7 +4822,7 @@
     <row r="27" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="32"/>
       <c r="B27" s="50" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>41</v>
@@ -4834,15 +4831,15 @@
         <v>1</v>
       </c>
       <c r="E27" s="44">
-        <v>45895</v>
+        <v>45899</v>
       </c>
       <c r="F27" s="44">
-        <v>45899</v>
+        <v>45902</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
@@ -4934,24 +4931,24 @@
     <row r="28" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="32"/>
       <c r="B28" s="50" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D28" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="44">
-        <v>45899</v>
+        <v>45902</v>
       </c>
       <c r="F28" s="44">
-        <v>45902</v>
+        <v>45908</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
@@ -5043,10 +5040,10 @@
     <row r="29" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="32"/>
       <c r="B29" s="50" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="13">
         <v>0</v>
@@ -5055,12 +5052,12 @@
         <v>45902</v>
       </c>
       <c r="F29" s="44">
-        <v>45908</v>
+        <v>45910</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
@@ -5152,25 +5149,22 @@
     <row r="30" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="32"/>
       <c r="B30" s="50" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D30" s="13">
         <v>0</v>
       </c>
       <c r="E30" s="44">
-        <v>45902</v>
+        <v>45909</v>
       </c>
       <c r="F30" s="44">
-        <v>45910</v>
+        <v>45916</v>
       </c>
       <c r="G30" s="12"/>
-      <c r="H30" s="12">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
+      <c r="H30" s="12"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
@@ -5261,19 +5255,19 @@
     <row r="31" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
       <c r="B31" s="50" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="13">
         <v>0</v>
       </c>
       <c r="E31" s="44">
-        <v>45909</v>
+        <v>45910</v>
       </c>
       <c r="F31" s="44">
-        <v>45916</v>
+        <v>45931</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -5367,19 +5361,19 @@
     <row r="32" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32"/>
       <c r="B32" s="50" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D32" s="13">
         <v>0</v>
       </c>
       <c r="E32" s="44">
-        <v>45910</v>
+        <v>45917</v>
       </c>
       <c r="F32" s="44">
-        <v>45931</v>
+        <v>45924</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
@@ -5470,7 +5464,7 @@
       <c r="CO32"/>
       <c r="CP32"/>
     </row>
-    <row r="33" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:94" s="3" customFormat="1" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="32"/>
       <c r="B33" s="50" t="s">
         <v>70</v>
@@ -5482,10 +5476,10 @@
         <v>0</v>
       </c>
       <c r="E33" s="44">
-        <v>45917</v>
+        <v>45925</v>
       </c>
       <c r="F33" s="44">
-        <v>45924</v>
+        <v>45931</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
@@ -5576,7 +5570,7 @@
       <c r="CO33"/>
       <c r="CP33"/>
     </row>
-    <row r="34" spans="1:94" s="3" customFormat="1" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32"/>
       <c r="B34" s="50" t="s">
         <v>71</v>
@@ -5588,10 +5582,10 @@
         <v>0</v>
       </c>
       <c r="E34" s="44">
-        <v>45925</v>
+        <v>45932</v>
       </c>
       <c r="F34" s="44">
-        <v>45931</v>
+        <v>45942</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -5682,13 +5676,13 @@
       <c r="CO34"/>
       <c r="CP34"/>
     </row>
-    <row r="35" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:94" s="3" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32"/>
       <c r="B35" s="50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="13">
         <v>0</v>
@@ -5788,7 +5782,7 @@
       <c r="CO35"/>
       <c r="CP35"/>
     </row>
-    <row r="36" spans="1:94" s="3" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:94" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32"/>
       <c r="B36" s="50" t="s">
         <v>75</v>
@@ -5800,10 +5794,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="44">
-        <v>45932</v>
+        <v>45942</v>
       </c>
       <c r="F36" s="44">
-        <v>45942</v>
+        <v>45945</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
@@ -5894,13 +5888,13 @@
       <c r="CO36"/>
       <c r="CP36"/>
     </row>
-    <row r="37" spans="1:94" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:94" s="3" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="32"/>
       <c r="B37" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D37" s="13">
         <v>0</v>
@@ -5909,7 +5903,7 @@
         <v>45942</v>
       </c>
       <c r="F37" s="44">
-        <v>45945</v>
+        <v>45950</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -6000,19 +5994,19 @@
       <c r="CO37"/>
       <c r="CP37"/>
     </row>
-    <row r="38" spans="1:94" s="3" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:94" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="32"/>
       <c r="B38" s="50" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D38" s="13">
         <v>0</v>
       </c>
       <c r="E38" s="44">
-        <v>45942</v>
+        <v>45945</v>
       </c>
       <c r="F38" s="44">
         <v>45950</v>
@@ -6106,22 +6100,22 @@
       <c r="CO38"/>
       <c r="CP38"/>
     </row>
-    <row r="39" spans="1:94" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:94" s="3" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="32"/>
       <c r="B39" s="50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D39" s="13">
         <v>0</v>
       </c>
       <c r="E39" s="44">
-        <v>45945</v>
+        <v>45950</v>
       </c>
       <c r="F39" s="44">
-        <v>45950</v>
+        <v>45960</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
@@ -6212,13 +6206,13 @@
       <c r="CO39"/>
       <c r="CP39"/>
     </row>
-    <row r="40" spans="1:94" s="3" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:94" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="32"/>
       <c r="B40" s="50" t="s">
         <v>79</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D40" s="13">
         <v>0</v>
@@ -6227,7 +6221,7 @@
         <v>45950</v>
       </c>
       <c r="F40" s="44">
-        <v>45960</v>
+        <v>45971</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
@@ -6318,9 +6312,9 @@
       <c r="CO40"/>
       <c r="CP40"/>
     </row>
-    <row r="41" spans="1:94" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:94" s="3" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="32"/>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="53" t="s">
         <v>80</v>
       </c>
       <c r="C41" s="39" t="s">
@@ -6330,10 +6324,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="44">
-        <v>45950</v>
+        <v>45971</v>
       </c>
       <c r="F41" s="44">
-        <v>45971</v>
+        <v>45991</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
@@ -6424,10 +6418,10 @@
       <c r="CO41"/>
       <c r="CP41"/>
     </row>
-    <row r="42" spans="1:94" s="3" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:94" s="3" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
-      <c r="B42" s="53" t="s">
-        <v>81</v>
+      <c r="B42" s="50" t="s">
+        <v>55</v>
       </c>
       <c r="C42" s="39" t="s">
         <v>41</v>
@@ -6436,10 +6430,10 @@
         <v>0</v>
       </c>
       <c r="E42" s="44">
-        <v>45971</v>
+        <v>46023</v>
       </c>
       <c r="F42" s="44">
-        <v>45991</v>
+        <v>46073</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
@@ -6530,23 +6524,19 @@
       <c r="CO42"/>
       <c r="CP42"/>
     </row>
-    <row r="43" spans="1:94" s="3" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="32"/>
-      <c r="B43" s="50" t="s">
-        <v>55</v>
+      <c r="B43" s="54" t="s">
+        <v>51</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D43" s="13">
         <v>0</v>
       </c>
-      <c r="E43" s="44">
-        <v>46023</v>
-      </c>
-      <c r="F43" s="44">
-        <v>46073</v>
-      </c>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="18"/>
@@ -6637,76 +6627,77 @@
       <c r="CP43"/>
     </row>
     <row r="44" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="13">
-        <v>0</v>
-      </c>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="18"/>
-      <c r="Z44" s="18"/>
-      <c r="AA44" s="18"/>
-      <c r="AB44" s="18"/>
-      <c r="AC44" s="18"/>
-      <c r="AD44" s="18"/>
-      <c r="AE44" s="18"/>
-      <c r="AF44" s="18"/>
-      <c r="AG44" s="18"/>
-      <c r="AH44" s="18"/>
-      <c r="AI44" s="18"/>
-      <c r="AJ44" s="18"/>
-      <c r="AK44" s="18"/>
-      <c r="AL44" s="18"/>
-      <c r="AM44" s="18"/>
-      <c r="AN44" s="18"/>
-      <c r="AO44" s="18"/>
-      <c r="AP44" s="18"/>
-      <c r="AQ44" s="18"/>
-      <c r="AR44" s="18"/>
-      <c r="AS44" s="18"/>
-      <c r="AT44" s="18"/>
-      <c r="AU44" s="18"/>
-      <c r="AV44" s="18"/>
-      <c r="AW44" s="18"/>
-      <c r="AX44" s="18"/>
-      <c r="AY44" s="18"/>
-      <c r="AZ44" s="18"/>
-      <c r="BA44" s="18"/>
-      <c r="BB44" s="18"/>
-      <c r="BC44" s="18"/>
-      <c r="BD44" s="18"/>
-      <c r="BE44" s="18"/>
-      <c r="BF44" s="18"/>
-      <c r="BG44" s="18"/>
-      <c r="BH44" s="18"/>
-      <c r="BI44" s="18"/>
-      <c r="BJ44" s="18"/>
-      <c r="BK44" s="18"/>
-      <c r="BL44" s="18"/>
+      <c r="A44" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="20"/>
+      <c r="AG44" s="20"/>
+      <c r="AH44" s="20"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="20"/>
+      <c r="AK44" s="20"/>
+      <c r="AL44" s="20"/>
+      <c r="AM44" s="20"/>
+      <c r="AN44" s="20"/>
+      <c r="AO44" s="20"/>
+      <c r="AP44" s="20"/>
+      <c r="AQ44" s="20"/>
+      <c r="AR44" s="20"/>
+      <c r="AS44" s="20"/>
+      <c r="AT44" s="20"/>
+      <c r="AU44" s="20"/>
+      <c r="AV44" s="20"/>
+      <c r="AW44" s="20"/>
+      <c r="AX44" s="20"/>
+      <c r="AY44" s="20"/>
+      <c r="AZ44" s="20"/>
+      <c r="BA44" s="20"/>
+      <c r="BB44" s="20"/>
+      <c r="BC44" s="20"/>
+      <c r="BD44" s="20"/>
+      <c r="BE44" s="20"/>
+      <c r="BF44" s="20"/>
+      <c r="BG44" s="20"/>
+      <c r="BH44" s="20"/>
+      <c r="BI44" s="20"/>
+      <c r="BJ44" s="20"/>
+      <c r="BK44" s="20"/>
+      <c r="BL44" s="20"/>
       <c r="BM44"/>
       <c r="BN44"/>
       <c r="BO44"/>
@@ -6738,134 +6729,31 @@
       <c r="CO44"/>
       <c r="CP44"/>
     </row>
-    <row r="45" spans="1:94" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="20"/>
-      <c r="Q45" s="20"/>
-      <c r="R45" s="20"/>
-      <c r="S45" s="20"/>
-      <c r="T45" s="20"/>
-      <c r="U45" s="20"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-      <c r="Y45" s="20"/>
-      <c r="Z45" s="20"/>
-      <c r="AA45" s="20"/>
-      <c r="AB45" s="20"/>
-      <c r="AC45" s="20"/>
-      <c r="AD45" s="20"/>
-      <c r="AE45" s="20"/>
-      <c r="AF45" s="20"/>
-      <c r="AG45" s="20"/>
-      <c r="AH45" s="20"/>
-      <c r="AI45" s="20"/>
-      <c r="AJ45" s="20"/>
-      <c r="AK45" s="20"/>
-      <c r="AL45" s="20"/>
-      <c r="AM45" s="20"/>
-      <c r="AN45" s="20"/>
-      <c r="AO45" s="20"/>
-      <c r="AP45" s="20"/>
-      <c r="AQ45" s="20"/>
-      <c r="AR45" s="20"/>
-      <c r="AS45" s="20"/>
-      <c r="AT45" s="20"/>
-      <c r="AU45" s="20"/>
-      <c r="AV45" s="20"/>
-      <c r="AW45" s="20"/>
-      <c r="AX45" s="20"/>
-      <c r="AY45" s="20"/>
-      <c r="AZ45" s="20"/>
-      <c r="BA45" s="20"/>
-      <c r="BB45" s="20"/>
-      <c r="BC45" s="20"/>
-      <c r="BD45" s="20"/>
-      <c r="BE45" s="20"/>
-      <c r="BF45" s="20"/>
-      <c r="BG45" s="20"/>
-      <c r="BH45" s="20"/>
-      <c r="BI45" s="20"/>
-      <c r="BJ45" s="20"/>
-      <c r="BK45" s="20"/>
-      <c r="BL45" s="20"/>
-      <c r="BM45"/>
-      <c r="BN45"/>
-      <c r="BO45"/>
-      <c r="BP45"/>
-      <c r="BQ45"/>
-      <c r="BR45"/>
-      <c r="BS45"/>
-      <c r="BT45"/>
-      <c r="BU45"/>
-      <c r="BV45"/>
-      <c r="BW45"/>
-      <c r="BX45"/>
-      <c r="BY45"/>
-      <c r="BZ45"/>
-      <c r="CA45"/>
-      <c r="CB45"/>
-      <c r="CC45"/>
-      <c r="CD45"/>
-      <c r="CE45"/>
-      <c r="CF45"/>
-      <c r="CG45"/>
-      <c r="CH45"/>
-      <c r="CI45"/>
-      <c r="CJ45"/>
-      <c r="CK45"/>
-      <c r="CL45"/>
-      <c r="CM45"/>
-      <c r="CN45"/>
-      <c r="CO45"/>
-      <c r="CP45"/>
+    <row r="45" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G46" s="6"/>
+      <c r="C46" s="10"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="10"/>
-      <c r="F47" s="34"/>
-    </row>
-    <row r="48" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="11"/>
+      <c r="C47" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D45">
+  <conditionalFormatting sqref="D7:D44">
     <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6879,12 +6767,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL45">
+  <conditionalFormatting sqref="I5:BL44">
     <cfRule type="expression" dxfId="2" priority="45">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL45">
+  <conditionalFormatting sqref="I7:BL44">
     <cfRule type="expression" dxfId="1" priority="39">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -6952,7 +6840,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D45</xm:sqref>
+          <xm:sqref>D7:D44</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7066,24 +6954,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
-    <_activity xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EDB812BAF41ADA4394A8076EA0B61C5B" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2edf200c4005839e532231d45070b11f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1386928-745a-4956-98a1-a16a4dd5b026" xmlns:ns4="135f4629-4c69-42bd-b907-0ef6c8daac89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbaa874e3aed9a9139054fcecbe44b3c" ns3:_="" ns4:_="">
     <xsd:import namespace="a1386928-745a-4956-98a1-a16a4dd5b026"/>
@@ -7330,10 +7200,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
+    <_activity xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7D7F31-B484-4E45-8243-CE827741D3B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1386928-745a-4956-98a1-a16a4dd5b026"/>
+    <ds:schemaRef ds:uri="135f4629-4c69-42bd-b907-0ef6c8daac89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7356,20 +7255,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7D7F31-B484-4E45-8243-CE827741D3B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1386928-745a-4956-98a1-a16a4dd5b026"/>
-    <ds:schemaRef ds:uri="135f4629-4c69-42bd-b907-0ef6c8daac89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Besprechungsprotokoll für den 22.09.2025 verfasst
</commit_message>
<xml_diff>
--- a/Projektplanung/Gantt-Diagramm.xlsx
+++ b/Projektplanung/Gantt-Diagramm.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485C174-EE1F-4D01-9755-40B17738470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E9DB9D-1E0B-4BCC-9CAF-1BA4DB79B020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57490" yWindow="-3540" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
@@ -1236,12 +1236,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1253,6 +1247,12 @@
     </xf>
     <xf numFmtId="169" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1646,7 +1646,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$E$4" horiz="1" max="100" page="0" val="12"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$E$4" horiz="1" max="100" page="0" val="4"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2046,8 +2046,8 @@
   <dimension ref="A1:CP47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2094,14 +2094,14 @@
       <c r="B3" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="60">
+      <c r="D3" s="60"/>
+      <c r="E3" s="58">
         <v>45819</v>
       </c>
-      <c r="F3" s="60"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:94" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -2110,93 +2110,93 @@
       <c r="B4" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="7">
-        <v>12</v>
-      </c>
-      <c r="I4" s="57">
+        <v>4</v>
+      </c>
+      <c r="I4" s="55">
         <f>I5</f>
-        <v>45894</v>
-      </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="57">
+        <v>45838</v>
+      </c>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="55">
         <f>P5</f>
-        <v>45901</v>
-      </c>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="57">
+        <v>45845</v>
+      </c>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="55">
         <f>W5</f>
-        <v>45908</v>
-      </c>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="57">
+        <v>45852</v>
+      </c>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="56"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="55">
         <f>AD5</f>
-        <v>45915</v>
-      </c>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="57">
+        <v>45859</v>
+      </c>
+      <c r="AE4" s="56"/>
+      <c r="AF4" s="56"/>
+      <c r="AG4" s="56"/>
+      <c r="AH4" s="56"/>
+      <c r="AI4" s="56"/>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="55">
         <f>AK5</f>
-        <v>45922</v>
-      </c>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="58"/>
-      <c r="AN4" s="58"/>
-      <c r="AO4" s="58"/>
-      <c r="AP4" s="58"/>
-      <c r="AQ4" s="59"/>
-      <c r="AR4" s="57">
+        <v>45866</v>
+      </c>
+      <c r="AL4" s="56"/>
+      <c r="AM4" s="56"/>
+      <c r="AN4" s="56"/>
+      <c r="AO4" s="56"/>
+      <c r="AP4" s="56"/>
+      <c r="AQ4" s="57"/>
+      <c r="AR4" s="55">
         <f>AR5</f>
-        <v>45929</v>
-      </c>
-      <c r="AS4" s="58"/>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="58"/>
-      <c r="AV4" s="58"/>
-      <c r="AW4" s="58"/>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="57">
+        <v>45873</v>
+      </c>
+      <c r="AS4" s="56"/>
+      <c r="AT4" s="56"/>
+      <c r="AU4" s="56"/>
+      <c r="AV4" s="56"/>
+      <c r="AW4" s="56"/>
+      <c r="AX4" s="57"/>
+      <c r="AY4" s="55">
         <f>AY5</f>
-        <v>45936</v>
-      </c>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="58"/>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="58"/>
-      <c r="BD4" s="58"/>
-      <c r="BE4" s="59"/>
-      <c r="BF4" s="57">
+        <v>45880</v>
+      </c>
+      <c r="AZ4" s="56"/>
+      <c r="BA4" s="56"/>
+      <c r="BB4" s="56"/>
+      <c r="BC4" s="56"/>
+      <c r="BD4" s="56"/>
+      <c r="BE4" s="57"/>
+      <c r="BF4" s="55">
         <f>BF5</f>
-        <v>45943</v>
-      </c>
-      <c r="BG4" s="58"/>
-      <c r="BH4" s="58"/>
-      <c r="BI4" s="58"/>
-      <c r="BJ4" s="58"/>
-      <c r="BK4" s="58"/>
-      <c r="BL4" s="59"/>
+        <v>45887</v>
+      </c>
+      <c r="BG4" s="56"/>
+      <c r="BH4" s="56"/>
+      <c r="BI4" s="56"/>
+      <c r="BJ4" s="56"/>
+      <c r="BK4" s="56"/>
+      <c r="BL4" s="57"/>
     </row>
     <row r="5" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -2210,227 +2210,227 @@
       <c r="G5" s="40"/>
       <c r="I5" s="47">
         <f>Projektanfang-WEEKDAY(Projektanfang,1)+2+7*(Anzeigewoche-1)</f>
-        <v>45894</v>
+        <v>45838</v>
       </c>
       <c r="J5" s="48">
         <f>I5+1</f>
-        <v>45895</v>
+        <v>45839</v>
       </c>
       <c r="K5" s="48">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>45896</v>
+        <v>45840</v>
       </c>
       <c r="L5" s="48">
         <f t="shared" si="0"/>
-        <v>45897</v>
+        <v>45841</v>
       </c>
       <c r="M5" s="48">
         <f t="shared" si="0"/>
-        <v>45898</v>
+        <v>45842</v>
       </c>
       <c r="N5" s="48">
         <f t="shared" si="0"/>
-        <v>45899</v>
+        <v>45843</v>
       </c>
       <c r="O5" s="49">
         <f t="shared" si="0"/>
-        <v>45900</v>
+        <v>45844</v>
       </c>
       <c r="P5" s="47">
         <f>O5+1</f>
-        <v>45901</v>
+        <v>45845</v>
       </c>
       <c r="Q5" s="48">
         <f>P5+1</f>
-        <v>45902</v>
+        <v>45846</v>
       </c>
       <c r="R5" s="48">
         <f t="shared" si="0"/>
-        <v>45903</v>
+        <v>45847</v>
       </c>
       <c r="S5" s="48">
         <f t="shared" si="0"/>
-        <v>45904</v>
+        <v>45848</v>
       </c>
       <c r="T5" s="48">
         <f t="shared" si="0"/>
-        <v>45905</v>
+        <v>45849</v>
       </c>
       <c r="U5" s="48">
         <f t="shared" si="0"/>
-        <v>45906</v>
+        <v>45850</v>
       </c>
       <c r="V5" s="49">
         <f t="shared" si="0"/>
-        <v>45907</v>
+        <v>45851</v>
       </c>
       <c r="W5" s="47">
         <f>V5+1</f>
-        <v>45908</v>
+        <v>45852</v>
       </c>
       <c r="X5" s="48">
         <f>W5+1</f>
-        <v>45909</v>
+        <v>45853</v>
       </c>
       <c r="Y5" s="48">
         <f t="shared" si="0"/>
-        <v>45910</v>
+        <v>45854</v>
       </c>
       <c r="Z5" s="48">
         <f t="shared" si="0"/>
-        <v>45911</v>
+        <v>45855</v>
       </c>
       <c r="AA5" s="48">
         <f t="shared" si="0"/>
-        <v>45912</v>
+        <v>45856</v>
       </c>
       <c r="AB5" s="48">
         <f t="shared" si="0"/>
-        <v>45913</v>
+        <v>45857</v>
       </c>
       <c r="AC5" s="49">
         <f t="shared" si="0"/>
-        <v>45914</v>
+        <v>45858</v>
       </c>
       <c r="AD5" s="47">
         <f>AC5+1</f>
-        <v>45915</v>
+        <v>45859</v>
       </c>
       <c r="AE5" s="48">
         <f>AD5+1</f>
-        <v>45916</v>
+        <v>45860</v>
       </c>
       <c r="AF5" s="48">
         <f t="shared" si="0"/>
-        <v>45917</v>
+        <v>45861</v>
       </c>
       <c r="AG5" s="48">
         <f t="shared" si="0"/>
-        <v>45918</v>
+        <v>45862</v>
       </c>
       <c r="AH5" s="48">
         <f t="shared" si="0"/>
-        <v>45919</v>
+        <v>45863</v>
       </c>
       <c r="AI5" s="48">
         <f t="shared" si="0"/>
-        <v>45920</v>
+        <v>45864</v>
       </c>
       <c r="AJ5" s="49">
         <f t="shared" si="0"/>
-        <v>45921</v>
+        <v>45865</v>
       </c>
       <c r="AK5" s="47">
         <f>AJ5+1</f>
-        <v>45922</v>
+        <v>45866</v>
       </c>
       <c r="AL5" s="48">
         <f>AK5+1</f>
-        <v>45923</v>
+        <v>45867</v>
       </c>
       <c r="AM5" s="48">
         <f t="shared" si="0"/>
-        <v>45924</v>
+        <v>45868</v>
       </c>
       <c r="AN5" s="48">
         <f t="shared" si="0"/>
-        <v>45925</v>
+        <v>45869</v>
       </c>
       <c r="AO5" s="48">
         <f t="shared" si="0"/>
-        <v>45926</v>
+        <v>45870</v>
       </c>
       <c r="AP5" s="48">
         <f t="shared" si="0"/>
-        <v>45927</v>
+        <v>45871</v>
       </c>
       <c r="AQ5" s="49">
         <f t="shared" si="0"/>
-        <v>45928</v>
+        <v>45872</v>
       </c>
       <c r="AR5" s="47">
         <f>AQ5+1</f>
-        <v>45929</v>
+        <v>45873</v>
       </c>
       <c r="AS5" s="48">
         <f>AR5+1</f>
-        <v>45930</v>
+        <v>45874</v>
       </c>
       <c r="AT5" s="48">
         <f t="shared" si="0"/>
-        <v>45931</v>
+        <v>45875</v>
       </c>
       <c r="AU5" s="48">
         <f t="shared" si="0"/>
-        <v>45932</v>
+        <v>45876</v>
       </c>
       <c r="AV5" s="48">
         <f t="shared" si="0"/>
-        <v>45933</v>
+        <v>45877</v>
       </c>
       <c r="AW5" s="48">
         <f t="shared" si="0"/>
-        <v>45934</v>
+        <v>45878</v>
       </c>
       <c r="AX5" s="49">
         <f t="shared" si="0"/>
-        <v>45935</v>
+        <v>45879</v>
       </c>
       <c r="AY5" s="47">
         <f>AX5+1</f>
-        <v>45936</v>
+        <v>45880</v>
       </c>
       <c r="AZ5" s="48">
         <f>AY5+1</f>
-        <v>45937</v>
+        <v>45881</v>
       </c>
       <c r="BA5" s="48">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45938</v>
+        <v>45882</v>
       </c>
       <c r="BB5" s="48">
         <f t="shared" si="1"/>
-        <v>45939</v>
+        <v>45883</v>
       </c>
       <c r="BC5" s="48">
         <f t="shared" si="1"/>
-        <v>45940</v>
+        <v>45884</v>
       </c>
       <c r="BD5" s="48">
         <f t="shared" si="1"/>
-        <v>45941</v>
+        <v>45885</v>
       </c>
       <c r="BE5" s="49">
         <f t="shared" si="1"/>
-        <v>45942</v>
+        <v>45886</v>
       </c>
       <c r="BF5" s="47">
         <f>BE5+1</f>
-        <v>45943</v>
+        <v>45887</v>
       </c>
       <c r="BG5" s="48">
         <f>BF5+1</f>
-        <v>45944</v>
+        <v>45888</v>
       </c>
       <c r="BH5" s="48">
         <f t="shared" ref="BH5:BK5" si="2">BG5+1</f>
-        <v>45945</v>
+        <v>45889</v>
       </c>
       <c r="BI5" s="48">
         <f t="shared" si="2"/>
-        <v>45946</v>
+        <v>45890</v>
       </c>
       <c r="BJ5" s="48">
         <f t="shared" si="2"/>
-        <v>45947</v>
+        <v>45891</v>
       </c>
       <c r="BK5" s="48">
         <f t="shared" si="2"/>
-        <v>45948</v>
+        <v>45892</v>
       </c>
       <c r="BL5" s="49">
         <f>BK5+1</f>
-        <v>45949</v>
+        <v>45893</v>
       </c>
     </row>
     <row r="6" spans="1:94" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6741,17 +6741,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D44">
     <cfRule type="dataBar" priority="26">
@@ -6954,6 +6954,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
+    <_activity xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EDB812BAF41ADA4394A8076EA0B61C5B" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2edf200c4005839e532231d45070b11f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1386928-745a-4956-98a1-a16a4dd5b026" xmlns:ns4="135f4629-4c69-42bd-b907-0ef6c8daac89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbaa874e3aed9a9139054fcecbe44b3c" ns3:_="" ns4:_="">
     <xsd:import namespace="a1386928-745a-4956-98a1-a16a4dd5b026"/>
@@ -7200,39 +7218,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
-    <_activity xmlns="a1386928-745a-4956-98a1-a16a4dd5b026" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7D7F31-B484-4E45-8243-CE827741D3B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1386928-745a-4956-98a1-a16a4dd5b026"/>
-    <ds:schemaRef ds:uri="135f4629-4c69-42bd-b907-0ef6c8daac89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7255,9 +7244,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D7D7F31-B484-4E45-8243-CE827741D3B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1386928-745a-4956-98a1-a16a4dd5b026"/>
+    <ds:schemaRef ds:uri="135f4629-4c69-42bd-b907-0ef6c8daac89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>